<commit_message>
api Post and setup relationship
</commit_message>
<xml_diff>
--- a/DienDanSV.xlsx
+++ b/DienDanSV.xlsx
@@ -1216,16 +1216,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>240030</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>67310</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>157480</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:colOff>891540</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1233,13 +1233,13 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="5673725" y="4392295"/>
-          <a:ext cx="613410" cy="741680"/>
+        <a:xfrm flipV="1">
+          <a:off x="6209030" y="4526280"/>
+          <a:ext cx="876300" cy="678180"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 50072"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1417,15 +1417,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>61595</xdr:colOff>
+      <xdr:colOff>84455</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>141605</xdr:rowOff>
+      <xdr:rowOff>164465</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1433195</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>73660</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1434,7 +1434,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3778250" y="324485"/>
+          <a:off x="3801110" y="347345"/>
           <a:ext cx="4808855" cy="823595"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
@@ -1856,8 +1856,8 @@
   <sheetPr/>
   <dimension ref="C1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>